<commit_message>
Corrections for Special Series
</commit_message>
<xml_diff>
--- a/src/Samples/Special/MasterTemplateV2.xlsx
+++ b/src/Samples/Special/MasterTemplateV2.xlsx
@@ -1374,8 +1374,8 @@
   </sheetPr>
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="106" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1515,7 @@
         <v>8</v>
       </c>
       <c r="G11" s="19">
-        <v>44965</v>
+        <v>44970</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -1547,7 +1547,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="20">
-        <v>44990</v>
+        <v>44997</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="10">
-        <f>ROUND(F16*E16*3,0)</f>
+        <f>ROUND(F16*E16,0)</f>
         <v>0</v>
       </c>
       <c r="H16" s="1"/>

</xml_diff>